<commit_message>
Chỉnh sửa và hoàn thành xong file report.xlsx
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t xml:space="preserve">Top 5 công nghệ đang được các doanh nghiệp ưu tiên đầu tư, ứng dụng cho hoạt động của doanh nghiệp </t>
   </si>
@@ -87,11 +87,44 @@
   <si>
     <t>Phản Hồi Chuyên Gia</t>
   </si>
+  <si>
+    <t>Top 5 Doanh Nghiệp Công Nghệ Việt Nam Uy Tín Trong Lĩnh Vực Dịch Vụ Công Nghệ Thông Tin Và Viễn Thông</t>
+  </si>
+  <si>
+    <t>FPT Corp</t>
+  </si>
+  <si>
+    <t>Viettel Group</t>
+  </si>
+  <si>
+    <t>VNPT Group</t>
+  </si>
+  <si>
+    <t>CMC Corp</t>
+  </si>
+  <si>
+    <t>VNG Corp</t>
+  </si>
+  <si>
+    <t>Tên Doanh Nghiệp</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -173,32 +206,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0%"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -237,6 +282,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -253,12 +301,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -564,11 +606,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="259596672"/>
-        <c:axId val="259598208"/>
+        <c:axId val="184738560"/>
+        <c:axId val="184740096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="259596672"/>
+        <c:axId val="184738560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,14 +619,15 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="259598208"/>
+        <c:crossAx val="184740096"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="259598208"/>
+        <c:axId val="184740096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,7 +637,8 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="259596672"/>
+        <c:crossAx val="184738560"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -734,6 +778,23 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="185381248"/>
+        <c:axId val="185382784"/>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
@@ -772,7 +833,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$21:$E$23</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.66700000000000004</c:v>
@@ -797,11 +858,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="151520768"/>
-        <c:axId val="210455552"/>
+        <c:axId val="190234624"/>
+        <c:axId val="188984704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151520768"/>
+        <c:axId val="185381248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,7 +871,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210455552"/>
+        <c:crossAx val="185382784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -818,7 +879,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210455552"/>
+        <c:axId val="185382784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -829,14 +890,45 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151520768"/>
+        <c:crossAx val="185381248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="188984704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="190234624"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="190234624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="188984704"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:pattFill prst="pct5">
           <a:fgClr>
-            <a:schemeClr val="accent1"/>
+            <a:schemeClr val="bg1"/>
           </a:fgClr>
           <a:bgClr>
             <a:schemeClr val="bg1"/>
@@ -849,14 +941,6 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:pattFill prst="pct20">
-      <a:fgClr>
-        <a:schemeClr val="accent1"/>
-      </a:fgClr>
-      <a:bgClr>
-        <a:schemeClr val="bg1"/>
-      </a:bgClr>
-    </a:pattFill>
     <a:ln w="6350">
       <a:solidFill>
         <a:schemeClr val="tx1">
@@ -982,6 +1066,23 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="120"/>
+        <c:overlap val="100"/>
+        <c:axId val="185272960"/>
+        <c:axId val="185274752"/>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
@@ -1060,15 +1161,15 @@
             <c:numRef>
               <c:f>Sheet1!$E$44:$E$46</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0" formatCode="0.00%">
+                <c:pt idx="0">
                   <c:v>0.875</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0.00%">
+                <c:pt idx="2">
                   <c:v>0.875</c:v>
                 </c:pt>
               </c:numCache>
@@ -1085,11 +1186,11 @@
         </c:dLbls>
         <c:gapWidth val="120"/>
         <c:overlap val="100"/>
-        <c:axId val="259439232"/>
-        <c:axId val="259528192"/>
+        <c:axId val="12246016"/>
+        <c:axId val="125047552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="259439232"/>
+        <c:axId val="185272960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1098,7 +1199,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="259528192"/>
+        <c:crossAx val="185274752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1106,7 +1207,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="259528192"/>
+        <c:axId val="185274752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1117,11 +1218,397 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="259439232"/>
+        <c:crossAx val="185272960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="125047552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="12246016"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="12246016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="125047552"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$69</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$70:$B$74</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>FPT Corp</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Viettel Group</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>VNPT Group</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CMC Corp</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>VNG Corp</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$70:$C$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$69</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$70:$B$74</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>FPT Corp</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Viettel Group</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>VNPT Group</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CMC Corp</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>VNG Corp</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$70:$D$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$69</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tỷ Lệ Phần Trăm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="66000"/>
+                      <a:satMod val="160000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="44500"/>
+                      <a:satMod val="160000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="23500"/>
+                      <a:satMod val="160000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="2700000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow>
+                <a:schemeClr val="accent1"/>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$70:$B$74</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>FPT Corp</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Viettel Group</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>VNPT Group</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>CMC Corp</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>VNG Corp</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$70:$E$74</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.161</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.161</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5999999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="206170368"/>
+        <c:axId val="206427264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="206170368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="206427264"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="206427264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="206170368"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="pct50">
+          <a:fgClr>
+            <a:schemeClr val="bg1"/>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:bgClr>
+        </a:pattFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1226,6 +1713,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2247900</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1304925</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1243,10 +1760,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A21:E23" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Phản hồi doanh nghiệp" headerRowDxfId="3"/>
-    <tableColumn id="3" name="Column2" headerRowDxfId="2"/>
-    <tableColumn id="4" name="Column3" headerRowDxfId="4"/>
-    <tableColumn id="5" name="Tỷ lệ phần trăm" dataDxfId="5"/>
+    <tableColumn id="2" name="Phản hồi doanh nghiệp" headerRowDxfId="7"/>
+    <tableColumn id="3" name="Column2" headerRowDxfId="6"/>
+    <tableColumn id="4" name="Column3" headerRowDxfId="5"/>
+    <tableColumn id="5" name="Tỷ lệ phần trăm" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1256,10 +1773,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A44:E46" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2" dataDxfId="1"/>
+    <tableColumn id="2" name="Column2" dataDxfId="4"/>
     <tableColumn id="3" name="Column3"/>
     <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Tỷ lệ phần trăm" headerRowDxfId="0"/>
+    <tableColumn id="5" name="Tỷ lệ phần trăm" headerRowDxfId="3" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A69:E74" totalsRowShown="0">
+  <autoFilter ref="A69:E74"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Tên Doanh Nghiệp"/>
+    <tableColumn id="3" name="Column2"/>
+    <tableColumn id="4" name="Column3"/>
+    <tableColumn id="5" name="Tỷ Lệ Phần Trăm" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1520,7 +2051,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1528,79 +2059,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="64" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" customWidth="1"/>
     <col min="7" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
       <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
         <v>0.78</v>
       </c>
     </row>
@@ -1608,11 +2139,11 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
         <v>0.78</v>
       </c>
     </row>
@@ -1623,8 +2154,8 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
         <v>0.67</v>
       </c>
     </row>
@@ -1632,11 +2163,11 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
         <v>0.56000000000000005</v>
       </c>
     </row>
@@ -1644,24 +2175,24 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
         <v>0.67</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
@@ -1672,10 +2203,10 @@
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="10">
         <v>0.66700000000000004</v>
       </c>
     </row>
@@ -1683,10 +2214,10 @@
       <c r="A22">
         <v>2</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="10">
         <v>0.55600000000000005</v>
       </c>
     </row>
@@ -1694,20 +2225,20 @@
       <c r="A23">
         <v>3</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="10">
         <v>0.44400000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
@@ -1718,10 +2249,10 @@
       <c r="A44">
         <v>1</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="10">
         <v>0.875</v>
       </c>
     </row>
@@ -1729,10 +2260,10 @@
       <c r="A45">
         <v>2</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="10">
         <v>0.75</v>
       </c>
     </row>
@@ -1740,23 +2271,104 @@
       <c r="A46">
         <v>3</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="10">
         <v>0.875</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="67" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B67" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" t="s">
+        <v>24</v>
+      </c>
+      <c r="D69" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" s="10">
+        <v>0.161</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="10">
+        <v>0.20300000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="10">
+        <v>0.161</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>4</v>
+      </c>
+      <c r="B73" t="s">
+        <v>20</v>
+      </c>
+      <c r="E73" s="10">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>5</v>
+      </c>
+      <c r="B74" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="10">
+        <v>4.5999999999999999E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B67:E67"/>
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="B48:E48"/>
@@ -1821,10 +2433,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
thống kê doanh thu của các cường quốc
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cs\Documents\GitHub\Cong-Nghe-4.0\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="403"/>
   </bookViews>
@@ -10,6 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId2"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t xml:space="preserve">Top 5 công nghệ đang được các doanh nghiệp ưu tiên đầu tư, ứng dụng cho hoạt động của doanh nghiệp </t>
   </si>
@@ -117,13 +125,40 @@
   <si>
     <t>Column3</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Sum of Mỹ</t>
+  </si>
+  <si>
+    <t>Sum of Anh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of Trung Quốc </t>
+  </si>
+  <si>
+    <t>Sum of Nga</t>
+  </si>
+  <si>
+    <t>Sum of Canada</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Thống kê doanh thu của các nước hàng đầu nền công nghiệp 4.0 từ 2012 - 2016(tỉ USD)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -206,11 +241,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -226,23 +265,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.0%"/>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0%"/>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <font>
@@ -277,6 +314,9 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -316,7 +356,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -391,6 +431,27 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
               <c:f>Sheet1!$A$4:$B$8</c:f>
@@ -442,11 +503,37 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A61E-4DAF-A388-F10AC9A5F733}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
               <c:f>Sheet1!$A$4:$B$8</c:f>
@@ -498,6 +585,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A61E-4DAF-A388-F10AC9A5F733}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -528,7 +620,34 @@
                 </a:gradFill>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-A61E-4DAF-A388-F10AC9A5F733}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
               <c:f>Sheet1!$A$4:$B$8</c:f>
@@ -595,6 +714,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-A61E-4DAF-A388-F10AC9A5F733}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -616,6 +740,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -660,7 +785,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -733,6 +858,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1F9F-499C-9D43-59CD51347154}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -777,6 +907,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1F9F-499C-9D43-59CD51347154}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -847,6 +982,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1F9F-499C-9D43-59CD51347154}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -868,6 +1008,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -916,10 +1057,12 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="188984704"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -958,7 +1101,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1021,6 +1164,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AFC7-46F4-90E7-0C8EF751A275}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1065,6 +1213,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AFC7-46F4-90E7-0C8EF751A275}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1175,6 +1328,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AFC7-46F4-90E7-0C8EF751A275}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1196,6 +1354,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1244,10 +1403,12 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="125047552"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1267,7 +1428,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1353,6 +1514,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0607-410E-B915-2D244F442715}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1420,6 +1586,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0607-410E-B915-2D244F442715}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1538,6 +1709,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0607-410E-B915-2D244F442715}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1559,10 +1735,12 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="206427264"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1581,6 +1759,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="206170368"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -1746,6 +1925,291 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="43617.86047013889" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="5">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A2:F7" sheet="Sheet1" r:id="rId2"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Năm" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2012" maxValue="2016" count="5">
+        <n v="2012"/>
+        <n v="2013"/>
+        <n v="2014"/>
+        <n v="2015"/>
+        <n v="2016"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Mỹ" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="93" maxValue="107" count="5">
+        <n v="105"/>
+        <n v="99"/>
+        <n v="102"/>
+        <n v="107"/>
+        <n v="93"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Anh" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="91" maxValue="103" count="5">
+        <n v="91"/>
+        <n v="98"/>
+        <n v="100"/>
+        <n v="103"/>
+        <n v="96"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Trung Quốc " numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="92" maxValue="110" count="5">
+        <n v="110"/>
+        <n v="99"/>
+        <n v="102"/>
+        <n v="108"/>
+        <n v="92"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Nga" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="87" maxValue="113" count="5">
+        <n v="87"/>
+        <n v="95"/>
+        <n v="113"/>
+        <n v="106"/>
+        <n v="102"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Canada" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="105" maxValue="111" count="5">
+        <n v="105"/>
+        <n v="107"/>
+        <n v="108"/>
+        <n v="110"/>
+        <n v="111"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="5">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="B92:G98" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </colItems>
+  <dataFields count="5">
+    <dataField name="Sum of Mỹ" fld="1" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Anh" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Trung Quốc " fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Nga" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Canada" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A4:B8" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
@@ -1763,7 +2227,7 @@
     <tableColumn id="2" name="Phản hồi doanh nghiệp" headerRowDxfId="7"/>
     <tableColumn id="3" name="Column2" headerRowDxfId="6"/>
     <tableColumn id="4" name="Column3" headerRowDxfId="5"/>
-    <tableColumn id="5" name="Tỷ lệ phần trăm" dataDxfId="1"/>
+    <tableColumn id="5" name="Tỷ lệ phần trăm" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1773,10 +2237,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A44:E46" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2" dataDxfId="4"/>
+    <tableColumn id="2" name="Column2" dataDxfId="3"/>
     <tableColumn id="3" name="Column3"/>
     <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Tỷ lệ phần trăm" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="5" name="Tỷ lệ phần trăm" headerRowDxfId="2" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2051,7 +2515,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2059,10 +2523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M74"/>
+  <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2076,52 +2540,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
       <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2184,15 +2648,15 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
@@ -2206,7 +2670,7 @@
       <c r="B21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="4">
         <v>0.66700000000000004</v>
       </c>
     </row>
@@ -2217,7 +2681,7 @@
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="4">
         <v>0.55600000000000005</v>
       </c>
     </row>
@@ -2228,17 +2692,17 @@
       <c r="B23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="4">
         <v>0.44400000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
@@ -2252,7 +2716,7 @@
       <c r="B44" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="4">
         <v>0.875</v>
       </c>
     </row>
@@ -2263,7 +2727,7 @@
       <c r="B45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="4">
         <v>0.75</v>
       </c>
     </row>
@@ -2274,25 +2738,25 @@
       <c r="B46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="4">
         <v>0.875</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
     </row>
     <row r="67" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -2318,7 +2782,7 @@
       <c r="B70" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="10">
+      <c r="E70" s="4">
         <v>0.161</v>
       </c>
     </row>
@@ -2329,7 +2793,7 @@
       <c r="B71" t="s">
         <v>18</v>
       </c>
-      <c r="E71" s="10">
+      <c r="E71" s="4">
         <v>0.20300000000000001</v>
       </c>
     </row>
@@ -2340,7 +2804,7 @@
       <c r="B72" t="s">
         <v>19</v>
       </c>
-      <c r="E72" s="10">
+      <c r="E72" s="4">
         <v>0.161</v>
       </c>
     </row>
@@ -2351,7 +2815,7 @@
       <c r="B73" t="s">
         <v>20</v>
       </c>
-      <c r="E73" s="10">
+      <c r="E73" s="4">
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
@@ -2362,8 +2826,156 @@
       <c r="B74" t="s">
         <v>21</v>
       </c>
-      <c r="E74" s="10">
+      <c r="E74" s="4">
         <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>33</v>
+      </c>
+      <c r="B91" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D92" t="s">
+        <v>28</v>
+      </c>
+      <c r="E92" t="s">
+        <v>29</v>
+      </c>
+      <c r="F92" t="s">
+        <v>30</v>
+      </c>
+      <c r="G92" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="11">
+        <v>2012</v>
+      </c>
+      <c r="C93" s="12">
+        <v>105</v>
+      </c>
+      <c r="D93" s="12">
+        <v>91</v>
+      </c>
+      <c r="E93" s="12">
+        <v>110</v>
+      </c>
+      <c r="F93" s="12">
+        <v>87</v>
+      </c>
+      <c r="G93" s="12">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="11">
+        <v>2013</v>
+      </c>
+      <c r="C94" s="12">
+        <v>99</v>
+      </c>
+      <c r="D94" s="12">
+        <v>98</v>
+      </c>
+      <c r="E94" s="12">
+        <v>99</v>
+      </c>
+      <c r="F94" s="12">
+        <v>95</v>
+      </c>
+      <c r="G94" s="12">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="11">
+        <v>2014</v>
+      </c>
+      <c r="C95" s="12">
+        <v>102</v>
+      </c>
+      <c r="D95" s="12">
+        <v>100</v>
+      </c>
+      <c r="E95" s="12">
+        <v>102</v>
+      </c>
+      <c r="F95" s="12">
+        <v>113</v>
+      </c>
+      <c r="G95" s="12">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C96" s="12">
+        <v>107</v>
+      </c>
+      <c r="D96" s="12">
+        <v>103</v>
+      </c>
+      <c r="E96" s="12">
+        <v>108</v>
+      </c>
+      <c r="F96" s="12">
+        <v>106</v>
+      </c>
+      <c r="G96" s="12">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="11">
+        <v>2016</v>
+      </c>
+      <c r="C97" s="12">
+        <v>93</v>
+      </c>
+      <c r="D97" s="12">
+        <v>96</v>
+      </c>
+      <c r="E97" s="12">
+        <v>92</v>
+      </c>
+      <c r="F97" s="12">
+        <v>102</v>
+      </c>
+      <c r="G97" s="12">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C98" s="12">
+        <v>506</v>
+      </c>
+      <c r="D98" s="12">
+        <v>488</v>
+      </c>
+      <c r="E98" s="12">
+        <v>511</v>
+      </c>
+      <c r="F98" s="12">
+        <v>503</v>
+      </c>
+      <c r="G98" s="12">
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -2431,13 +3043,13 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
   <tableParts count="4">
-    <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
thống kê theo biểu đồ
doanh thu của các cường quốc hàng đầu trong nền công nghiệp 4.0
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="1" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t xml:space="preserve">Top 5 công nghệ đang được các doanh nghiệp ưu tiên đầu tư, ứng dụng cho hoạt động của doanh nghiệp </t>
   </si>
@@ -152,6 +152,9 @@
   <si>
     <t>Thống kê doanh thu của các nước hàng đầu nền công nghiệp 4.0 từ 2012 - 2016(tỉ USD)</t>
   </si>
+  <si>
+    <t>Thống kê theo biểu đồ</t>
+  </si>
 </sst>
 </file>
 
@@ -247,6 +250,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -265,11 +273,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1800,6 +1803,1235 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sum of Mỹ</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>2012</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2013</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>2014</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>2015</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>2016</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>105</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>99</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>102</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>107</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>93</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8191-4BCA-AD3C-9274EC70E481}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Sum of Anh</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>2012</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2013</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>2014</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>2015</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>2016</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>91</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>98</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>100</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>103</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>96</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8191-4BCA-AD3C-9274EC70E481}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Sum of Trung Quốc </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>2012</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2013</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>2014</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>2015</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>2016</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>110</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>99</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>102</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>108</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>92</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8191-4BCA-AD3C-9274EC70E481}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Sum of Nga</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>2012</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2013</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>2014</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>2015</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>2016</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>87</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>95</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>113</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>106</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>102</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8191-4BCA-AD3C-9274EC70E481}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Sum of Canada</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>2012</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2013</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>2014</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>2015</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>2016</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>105</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>107</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>108</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>110</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>111</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8191-4BCA-AD3C-9274EC70E481}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="314173808"/>
+        <c:axId val="314165968"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="314173808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="314165968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="314165968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="314173808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1917,6 +3149,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2040,7 +3304,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="B92:G98" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -2303,7 +3567,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2338,7 +3602,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2523,10 +3787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2540,52 +3804,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
     </row>
     <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
       <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2648,15 +3912,15 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
@@ -2697,12 +3961,12 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
@@ -2743,20 +4007,20 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
     </row>
     <row r="67" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -2839,10 +4103,10 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B92" s="13" t="s">
+      <c r="B92" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C92" s="13" t="s">
+      <c r="C92" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D92" t="s">
@@ -2859,123 +4123,128 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="11">
+      <c r="B93" s="5">
         <v>2012</v>
       </c>
-      <c r="C93" s="12">
+      <c r="C93" s="6">
         <v>105</v>
       </c>
-      <c r="D93" s="12">
+      <c r="D93" s="6">
         <v>91</v>
       </c>
-      <c r="E93" s="12">
+      <c r="E93" s="6">
         <v>110</v>
       </c>
-      <c r="F93" s="12">
+      <c r="F93" s="6">
         <v>87</v>
       </c>
-      <c r="G93" s="12">
+      <c r="G93" s="6">
         <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B94" s="11">
+      <c r="B94" s="5">
         <v>2013</v>
       </c>
-      <c r="C94" s="12">
+      <c r="C94" s="6">
         <v>99</v>
       </c>
-      <c r="D94" s="12">
+      <c r="D94" s="6">
         <v>98</v>
       </c>
-      <c r="E94" s="12">
+      <c r="E94" s="6">
         <v>99</v>
       </c>
-      <c r="F94" s="12">
+      <c r="F94" s="6">
         <v>95</v>
       </c>
-      <c r="G94" s="12">
+      <c r="G94" s="6">
         <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="11">
+      <c r="B95" s="5">
         <v>2014</v>
       </c>
-      <c r="C95" s="12">
+      <c r="C95" s="6">
         <v>102</v>
       </c>
-      <c r="D95" s="12">
+      <c r="D95" s="6">
         <v>100</v>
       </c>
-      <c r="E95" s="12">
+      <c r="E95" s="6">
         <v>102</v>
       </c>
-      <c r="F95" s="12">
+      <c r="F95" s="6">
         <v>113</v>
       </c>
-      <c r="G95" s="12">
+      <c r="G95" s="6">
         <v>108</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B96" s="11">
+      <c r="B96" s="5">
         <v>2015</v>
       </c>
-      <c r="C96" s="12">
+      <c r="C96" s="6">
         <v>107</v>
       </c>
-      <c r="D96" s="12">
+      <c r="D96" s="6">
         <v>103</v>
       </c>
-      <c r="E96" s="12">
+      <c r="E96" s="6">
         <v>108</v>
       </c>
-      <c r="F96" s="12">
+      <c r="F96" s="6">
         <v>106</v>
       </c>
-      <c r="G96" s="12">
+      <c r="G96" s="6">
         <v>110</v>
       </c>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="11">
+      <c r="B97" s="5">
         <v>2016</v>
       </c>
-      <c r="C97" s="12">
+      <c r="C97" s="6">
         <v>93</v>
       </c>
-      <c r="D97" s="12">
+      <c r="D97" s="6">
         <v>96</v>
       </c>
-      <c r="E97" s="12">
+      <c r="E97" s="6">
         <v>92</v>
       </c>
-      <c r="F97" s="12">
+      <c r="F97" s="6">
         <v>102</v>
       </c>
-      <c r="G97" s="12">
+      <c r="G97" s="6">
         <v>111</v>
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="11" t="s">
+      <c r="B98" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C98" s="12">
+      <c r="C98" s="6">
         <v>506</v>
       </c>
-      <c r="D98" s="12">
+      <c r="D98" s="6">
         <v>488</v>
       </c>
-      <c r="E98" s="12">
+      <c r="E98" s="6">
         <v>511</v>
       </c>
-      <c r="F98" s="12">
+      <c r="F98" s="6">
         <v>503</v>
       </c>
-      <c r="G98" s="12">
+      <c r="G98" s="6">
         <v>541</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>